<commit_message>
Nicer nav, added more components
</commit_message>
<xml_diff>
--- a/devtools-dashboard-mvp.xlsx
+++ b/devtools-dashboard-mvp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myownshit\devtools-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130FF48F-F5A0-4BD5-ABC6-7561514793B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFD3A57-D0F6-4578-8C1B-0B118565D151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="1350" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -210,64 +210,11 @@
   <cellStyles count="1">
     <cellStyle name="Navadno" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
       <border>
@@ -343,44 +290,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
       <border>
@@ -703,7 +613,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +653,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -754,7 +664,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -765,7 +675,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -776,7 +686,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -787,7 +697,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -798,7 +708,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -809,7 +719,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -831,7 +741,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -891,21 +801,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C16">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>"DONE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"PENDING"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"TO DO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"DONE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"PENDING"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>